<commit_message>
Partial update of RF cavity
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/CylindricalRFcavity.xlsx
+++ b/21-Spreads4Tests/CylindricalRFcavity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4399A1BF-2F90-A24F-8A36-B64A8ECFFB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311763A2-81BD-AA49-A1A1-5B079CAEF615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
@@ -687,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -723,6 +723,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -738,51 +763,15 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1099,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210C9CAF-347D-914C-A112-6F8981E6D7C0}">
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1115,54 +1104,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="24" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3">
         <f>H9</f>
         <v>1</v>
       </c>
-      <c r="C3" s="35"/>
       <c r="D3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3">
         <v>4</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="22" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="8">
@@ -1176,23 +1164,23 @@
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="21">
         <f>H9*B5</f>
         <v>1.6021766339999999E-19</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4">
         <v>200</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="8">
@@ -1207,22 +1195,22 @@
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="21">
         <v>1.6021766339999999E-19</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="22" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="8">
@@ -1237,16 +1225,15 @@
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="11">
         <v>299792458</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" s="35"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="23" t="s">
         <v>7</v>
       </c>
       <c r="H6">
@@ -1256,17 +1243,17 @@
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="29" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="40" t="s">
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="23" t="s">
         <v>12</v>
       </c>
       <c r="H7">
@@ -1279,23 +1266,23 @@
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8">
         <v>938.27208815999995</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8">
         <f>2*PI()*E4</f>
         <v>1256.6370614359173</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="23" t="s">
         <v>11</v>
       </c>
       <c r="H8">
@@ -1311,14 +1298,14 @@
       <c r="D9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9">
         <f>(E8*10^6)/B6</f>
         <v>4.191690043903364</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H9">
@@ -1330,7 +1317,7 @@
       <c r="D10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10">
         <f>PI()*H7*B6/(E8*10^6)</f>
         <v>0.15232400590198045</v>
       </c>
@@ -1345,7 +1332,7 @@
       <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11">
         <f>2.4048/E9</f>
         <v>0.57370654194664983</v>
       </c>
@@ -1357,7 +1344,7 @@
       <c r="D12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12">
         <f>(2*PI()*H7)/(E9^2*E10^2)*SIN(E9*E10/2/H7)</f>
         <v>3.1323658611678535</v>
       </c>
@@ -1368,7 +1355,7 @@
       <c r="D13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13">
         <f>E10*E3*E12</f>
         <v>1.9085380636947769</v>
       </c>
@@ -1380,24 +1367,23 @@
       <c r="D14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="35">
-        <f>E3/H5</f>
-        <v>2.0538253590784612E-2</v>
+      <c r="E14">
+        <f>E13/H5/1000</f>
+        <v>9.7995096849570887E-6</v>
       </c>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D15" s="20"/>
-      <c r="E15" s="35"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D16" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16">
         <f>E9*SQRT(E14*COS(E5)/2/PI())</f>
-        <v>0.2396519586924635</v>
+        <v>5.2348157468855641E-3</v>
       </c>
       <c r="F16" s="4"/>
     </row>
@@ -1405,49 +1391,47 @@
       <c r="D17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17">
         <f>E9*SQRT(E14*COS(E6)/PI())/H6</f>
-        <v>1.6327823545809175</v>
+        <v>3.566553274853692E-2</v>
       </c>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D18" s="20"/>
-      <c r="E18" s="35"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="2:7" ht="18" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19">
         <f>COS(E16*E10)</f>
-        <v>0.9993337757351608</v>
+        <v>0.99999968208612211</v>
       </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="2:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20">
         <f>SIN(E16*E10)/E16</f>
-        <v>0.15229017708302034</v>
+        <v>0.1523239897600083</v>
       </c>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D21" s="3"/>
-      <c r="E21" s="35"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="2:7" ht="18" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="35">
+      <c r="E22">
         <f>COS(E17*E10)</f>
-        <v>0.96923028678649281</v>
+        <v>0.99998524283026791</v>
       </c>
       <c r="F22" s="4"/>
     </row>
@@ -1455,9 +1439,9 @@
       <c r="D23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23">
         <f>SIN(E17*E10)/E17</f>
-        <v>0.15075845539350044</v>
+        <v>0.15232325661084017</v>
       </c>
       <c r="F23" s="4"/>
     </row>
@@ -1467,23 +1451,23 @@
       <c r="F24" s="6"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="18">
         <f>E19</f>
-        <v>0.9993337757351608</v>
+        <v>0.99999968208612211</v>
       </c>
       <c r="C29" s="2">
         <f>E20</f>
-        <v>0.15229017708302034</v>
+        <v>0.1523239897600083</v>
       </c>
       <c r="D29" s="19">
         <v>0</v>
@@ -1501,19 +1485,19 @@
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="10">
         <f>-E20*E16^2</f>
-        <v>-8.7464910765788547E-3</v>
+        <v>-4.1741793646471644E-6</v>
       </c>
       <c r="C30" s="6">
         <f>E19</f>
-        <v>0.9993337757351608</v>
-      </c>
-      <c r="D30" s="35">
-        <v>0</v>
-      </c>
-      <c r="E30" s="35">
-        <v>0</v>
-      </c>
-      <c r="F30" s="35">
+        <v>0.99999968208612211</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
         <v>0</v>
       </c>
       <c r="G30" s="4">
@@ -1524,18 +1508,18 @@
       <c r="B31" s="20">
         <v>0</v>
       </c>
-      <c r="C31" s="35">
+      <c r="C31">
         <v>0</v>
       </c>
       <c r="D31" s="18">
         <f>E19</f>
-        <v>0.9993337757351608</v>
+        <v>0.99999968208612211</v>
       </c>
       <c r="E31" s="2">
         <f>E20</f>
-        <v>0.15229017708302034</v>
-      </c>
-      <c r="F31" s="35">
+        <v>0.1523239897600083</v>
+      </c>
+      <c r="F31">
         <v>0</v>
       </c>
       <c r="G31" s="4">
@@ -1546,18 +1530,18 @@
       <c r="B32" s="20">
         <v>0</v>
       </c>
-      <c r="C32" s="35">
+      <c r="C32">
         <v>0</v>
       </c>
       <c r="D32" s="10">
         <f>-E20*E16^2</f>
-        <v>-8.7464910765788547E-3</v>
+        <v>-4.1741793646471644E-6</v>
       </c>
       <c r="E32" s="6">
         <f>E19</f>
-        <v>0.9993337757351608</v>
-      </c>
-      <c r="F32" s="42">
+        <v>0.99999968208612211</v>
+      </c>
+      <c r="F32">
         <v>0</v>
       </c>
       <c r="G32" s="4">
@@ -1568,22 +1552,22 @@
       <c r="B33" s="20">
         <v>0</v>
       </c>
-      <c r="C33" s="35">
-        <v>0</v>
-      </c>
-      <c r="D33" s="35">
-        <v>0</v>
-      </c>
-      <c r="E33" s="42">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
         <v>0</v>
       </c>
       <c r="F33" s="18">
         <f>E22</f>
-        <v>0.96923028678649281</v>
+        <v>0.99998524283026791</v>
       </c>
       <c r="G33" s="2">
         <f>E23/H6^2</f>
-        <v>3.4990191105889763</v>
+        <v>3.5353372683298034</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1601,11 +1585,11 @@
       </c>
       <c r="F34" s="10">
         <f>E23*E17^2*H6^2</f>
-        <v>1.7317039221764509E-2</v>
+        <v>8.348318547887133E-6</v>
       </c>
       <c r="G34" s="6">
         <f>E22</f>
-        <v>0.96923028678649281</v>
+        <v>0.99998524283026791</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1620,14 +1604,14 @@
       </c>
       <c r="E36" s="15">
         <f t="array" ref="E36:E41">MMULT(B29:G34,B36:B41)</f>
-        <v>0.51489590557588238</v>
+        <v>0.51523224001906187</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>23</v>
       </c>
       <c r="H36" s="15">
         <f>B29*B$36+C29*B$37+D29*B$38+E29*B$39+F29*B$40+G29*B$41</f>
-        <v>0.51489590557588238</v>
+        <v>0.51523224001906187</v>
       </c>
       <c r="J36" s="14" t="s">
         <v>25</v>
@@ -1642,11 +1626,11 @@
         <v>0.1</v>
       </c>
       <c r="E37" s="16">
-        <v>9.5560132035226661E-2</v>
+        <v>9.9997881118929891E-2</v>
       </c>
       <c r="H37" s="16">
         <f t="shared" ref="H37:H41" si="0">B30*B$36+C30*B$37+D30*B$38+E30*B$39+F30*B$40+G30*B$41</f>
-        <v>9.5560132035226661E-2</v>
+        <v>9.9997881118929891E-2</v>
       </c>
       <c r="K37" s="16">
         <f t="shared" ref="K37:K41" si="1">E37-H37</f>
@@ -1659,11 +1643,11 @@
         <v>-0.3</v>
       </c>
       <c r="E38" s="16">
-        <v>-0.33025816813715231</v>
+        <v>-0.33046470257783833</v>
       </c>
       <c r="H38" s="16">
         <f t="shared" si="0"/>
-        <v>-0.33025816813715231</v>
+        <v>-0.33046470257783833</v>
       </c>
       <c r="K38" s="16">
         <f t="shared" si="1"/>
@@ -1675,11 +1659,11 @@
         <v>-0.2</v>
       </c>
       <c r="E39" s="16">
-        <v>-0.19724280782405851</v>
+        <v>-0.19999868416341504</v>
       </c>
       <c r="H39" s="16">
         <f t="shared" si="0"/>
-        <v>-0.19724280782405851</v>
+        <v>-0.19999868416341504</v>
       </c>
       <c r="K39" s="16">
         <f t="shared" si="1"/>
@@ -1687,15 +1671,15 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="43">
+      <c r="B40" s="16">
         <v>0.1</v>
       </c>
       <c r="E40" s="16">
-        <v>0.79672685079644467</v>
+        <v>0.80706597794898749</v>
       </c>
       <c r="H40" s="16">
         <f t="shared" si="0"/>
-        <v>0.79672685079644467</v>
+        <v>0.80706597794898749</v>
       </c>
       <c r="K40" s="16">
         <f t="shared" si="1"/>
@@ -1703,15 +1687,15 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="44">
+      <c r="B41" s="17">
         <v>0.2</v>
       </c>
       <c r="E41" s="17">
-        <v>0.19557776127947502</v>
+        <v>0.19999788339790839</v>
       </c>
       <c r="H41" s="17">
         <f t="shared" si="0"/>
-        <v>0.19557776127947502</v>
+        <v>0.19999788339790839</v>
       </c>
       <c r="K41" s="17">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Commit first version of RF cavity code
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/CylindricalRFcavity.xlsx
+++ b/21-Spreads4Tests/CylindricalRFcavity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311763A2-81BD-AA49-A1A1-5B079CAEF615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8A6069-8203-7E49-A9C0-EAB5E89E133C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="7140" yWindow="640" windowWidth="30240" windowHeight="18900" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>MeV</t>
   </si>
@@ -417,6 +417,22 @@
         <rFont val="Calibri (Body)"/>
       </rPr>
       <t>perp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>rf</t>
     </r>
   </si>
 </sst>
@@ -427,7 +443,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -494,6 +510,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -521,7 +545,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -683,11 +707,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -770,6 +809,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1088,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210C9CAF-347D-914C-A112-6F8981E6D7C0}">
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1333,8 +1384,8 @@
         <v>36</v>
       </c>
       <c r="E11">
-        <f>2.4048/E9</f>
-        <v>0.57370654194664983</v>
+        <f>2.40482556/E9</f>
+        <v>0.57371263972576336</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>17</v>
@@ -1387,7 +1438,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D17" s="9" t="s">
         <v>43</v>
       </c>
@@ -1397,11 +1448,11 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D18" s="20"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
         <v>48</v>
       </c>
@@ -1411,7 +1462,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D20" s="3" t="s">
         <v>47</v>
       </c>
@@ -1421,11 +1472,11 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D21" s="3"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
         <v>46</v>
       </c>
@@ -1435,7 +1486,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
         <v>45</v>
       </c>
@@ -1445,12 +1496,12 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D24" s="10"/>
       <c r="E24" s="5"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B28" s="27" t="s">
         <v>21</v>
       </c>
@@ -1459,8 +1510,11 @@
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="G28" s="29"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I28" s="38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="18">
         <f>E19</f>
         <v>0.99999968208612211</v>
@@ -1481,8 +1535,11 @@
       <c r="G29" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I29" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="10">
         <f>-E20*E16^2</f>
         <v>-4.1741793646471644E-6</v>
@@ -1503,8 +1560,11 @@
       <c r="G30" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I30" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="20">
         <v>0</v>
       </c>
@@ -1525,8 +1585,11 @@
       <c r="G31" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I31" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="20">
         <v>0</v>
       </c>
@@ -1547,6 +1610,9 @@
       <c r="G32" s="4">
         <v>0</v>
       </c>
+      <c r="I32" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B33" s="20">
@@ -1569,6 +1635,10 @@
         <f>E23/H6^2</f>
         <v>3.5353372683298034</v>
       </c>
+      <c r="I33" s="40">
+        <f>(1-E22)*TAN(E5)/E9</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B34" s="10">
@@ -1591,6 +1661,10 @@
         <f>E22</f>
         <v>0.99998524283026791</v>
       </c>
+      <c r="I34" s="41">
+        <f>H6^2*E17*E23*TAN(E5)/E9</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
@@ -1603,14 +1677,14 @@
         <v>22</v>
       </c>
       <c r="E36" s="15">
-        <f t="array" ref="E36:E41">MMULT(B29:G34,B36:B41)</f>
+        <f t="array" ref="E36:E41">MMULT(B29:G34,B36:B41)+I29:I34</f>
         <v>0.51523224001906187</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>23</v>
       </c>
       <c r="H36" s="15">
-        <f>B29*B$36+C29*B$37+D29*B$38+E29*B$39+F29*B$40+G29*B$41</f>
+        <f>B29*B$36+C29*B$37+D29*B$38+E29*B$39+F29*B$40+G29*B$41+I29</f>
         <v>0.51523224001906187</v>
       </c>
       <c r="J36" s="14" t="s">
@@ -1629,7 +1703,7 @@
         <v>9.9997881118929891E-2</v>
       </c>
       <c r="H37" s="16">
-        <f t="shared" ref="H37:H41" si="0">B30*B$36+C30*B$37+D30*B$38+E30*B$39+F30*B$40+G30*B$41</f>
+        <f t="shared" ref="H37:H41" si="0">B30*B$36+C30*B$37+D30*B$38+E30*B$39+F30*B$40+G30*B$41+I30</f>
         <v>9.9997881118929891E-2</v>
       </c>
       <c r="K37" s="16">

</xml_diff>

<commit_message>
Fix transit time factor
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/CylindricalRFcavity.xlsx
+++ b/21-Spreads4Tests/CylindricalRFcavity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEB0835-005B-9A43-9201-A6113B4195C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7C0D9F-0746-AA47-AFCA-2623524D2388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18120" yWindow="2460" windowWidth="30240" windowHeight="18900" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -247,9 +247,6 @@
     <t>Electric field gradient</t>
   </si>
   <si>
-    <t>kV/m</t>
-  </si>
-  <si>
     <t>Frequency</t>
   </si>
   <si>
@@ -295,9 +292,6 @@
     <t>Cavity length</t>
   </si>
   <si>
-    <t>kV</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -434,6 +428,12 @@
       </rPr>
       <t>rf</t>
     </r>
+  </si>
+  <si>
+    <t>MV/m</t>
+  </si>
+  <si>
+    <t>MV</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1140,7 @@
   <dimension ref="A1:K87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:E41"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1197,10 +1197,10 @@
         <v>30</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="G3" s="22" t="s">
         <v>4</v>
@@ -1224,13 +1224,13 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4">
         <v>200</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>5</v>
@@ -1254,13 +1254,13 @@
         <v>10</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>0.1</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>6</v>
@@ -1332,7 +1332,7 @@
         <v>1256.6370614359173</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="23" t="s">
         <v>11</v>
@@ -1348,14 +1348,14 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9">
         <f>(E8*10^6)/B6</f>
         <v>4.191690043903364</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>2</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10">
         <f>PI()*H7*B6/(E8*10^6)</f>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11">
         <f>2.40482556/E9</f>
@@ -1394,11 +1394,11 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12">
-        <f>(2*PI()*H7)/(E9^2*E10^2)*SIN(E9*E10/2/H7)</f>
-        <v>3.1323658611678535</v>
+        <f>(2*H7)/(E9*E10)*SIN(E9*E10/2/H7)</f>
+        <v>0.63661977236758138</v>
       </c>
       <c r="F12" s="4"/>
       <c r="H12" s="11"/>
@@ -1409,10 +1409,10 @@
       </c>
       <c r="E13">
         <f>E10*E3*E12</f>
-        <v>1.9085380636947769</v>
+        <v>1.9394494792687385</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="E14">
         <f>E13/H5/1000</f>
-        <v>9.7995096849570887E-6</v>
+        <v>9.9582263079341287E-6</v>
       </c>
       <c r="F14" s="4"/>
     </row>
@@ -1431,21 +1431,21 @@
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D16" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E16">
         <f>E9*SQRT(E14*COS(E5)/2/PI())</f>
-        <v>5.2217232372721682E-3</v>
+        <v>5.2638399054541216E-3</v>
       </c>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D17" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E17">
         <f>E9*SQRT(E14*COS(E5)/PI())/H6</f>
-        <v>3.5576331647112311E-2</v>
+        <v>3.5863278405304594E-2</v>
       </c>
       <c r="F17" s="4"/>
     </row>
@@ -1455,21 +1455,21 @@
     </row>
     <row r="19" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E19">
         <f>COS(E16*E10)</f>
-        <v>0.9999996836743672</v>
+        <v>0.999999678551036</v>
       </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D20" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E20">
         <f>SIN(E16*E10)/E16</f>
-        <v>0.1523239898406509</v>
+        <v>0.15232398958051549</v>
       </c>
       <c r="F20" s="4"/>
     </row>
@@ -1479,21 +1479,21 @@
     </row>
     <row r="22" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E22">
         <f>COS(E17*E10)</f>
-        <v>0.99998531655446843</v>
+        <v>0.99998507873633591</v>
       </c>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E23">
         <f>SIN(E17*E10)/E17</f>
-        <v>0.15232326035416935</v>
+        <v>0.15232324827900867</v>
       </c>
       <c r="F23" s="4"/>
     </row>
@@ -1512,17 +1512,17 @@
       <c r="F28" s="32"/>
       <c r="G28" s="33"/>
       <c r="I28" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="18">
         <f>E19</f>
-        <v>0.9999996836743672</v>
+        <v>0.999999678551036</v>
       </c>
       <c r="C29" s="2">
         <f>E20</f>
-        <v>0.1523239898406509</v>
+        <v>0.15232398958051549</v>
       </c>
       <c r="D29" s="19">
         <v>0</v>
@@ -1543,11 +1543,11 @@
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="10">
         <f>-E20*E16^2</f>
-        <v>-4.1533258566403462E-6</v>
+        <v>-4.2205947103532851E-6</v>
       </c>
       <c r="C30" s="6">
         <f>E19</f>
-        <v>0.9999996836743672</v>
+        <v>0.999999678551036</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1574,11 +1574,11 @@
       </c>
       <c r="D31" s="18">
         <f>E19</f>
-        <v>0.9999996836743672</v>
+        <v>0.999999678551036</v>
       </c>
       <c r="E31" s="2">
         <f>E20</f>
-        <v>0.1523239898406509</v>
+        <v>0.15232398958051549</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1599,11 +1599,11 @@
       </c>
       <c r="D32" s="10">
         <f>-E20*E16^2</f>
-        <v>-4.1533258566403462E-6</v>
+        <v>-4.2205947103532851E-6</v>
       </c>
       <c r="E32" s="6">
         <f>E19</f>
-        <v>0.9999996836743672</v>
+        <v>0.999999678551036</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1630,15 +1630,15 @@
       </c>
       <c r="F33" s="18">
         <f>E22</f>
-        <v>0.99998531655446843</v>
+        <v>0.99998507873633591</v>
       </c>
       <c r="G33" s="2">
         <f>E23/H6^2</f>
-        <v>3.535337355210372</v>
+        <v>3.5353370749526722</v>
       </c>
       <c r="I33" s="26">
         <f>(1-E22)*TAN(E5)/E9</f>
-        <v>3.5147128653693854E-7</v>
+        <v>3.5716383634202152E-7</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1656,15 +1656,15 @@
       </c>
       <c r="F34" s="10">
         <f>E23*E17^2*H6^2</f>
-        <v>8.3066119323496763E-6</v>
+        <v>8.4411483407266255E-6</v>
       </c>
       <c r="G34" s="6">
         <f>E22</f>
-        <v>0.99998531655446843</v>
+        <v>0.99998507873633591</v>
       </c>
       <c r="I34" s="27">
         <f>H6^2*E17*E23*TAN(E5)/E9</f>
-        <v>5.5888780215082712E-6</v>
+        <v>5.6339555904082248E-6</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1679,14 +1679,14 @@
       </c>
       <c r="E36" s="15">
         <f t="array" ref="E36:E41">MMULT(B29:G34,B36:B41)+I29:I34</f>
-        <v>0.51523224082124874</v>
+        <v>0.51523223823356956</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>23</v>
       </c>
       <c r="H36" s="15">
         <f>B29*B$36+C29*B$37+D29*B$38+E29*B$39+F29*B$40+G29*B$41+I29</f>
-        <v>0.51523224082124874</v>
+        <v>0.51523223823356956</v>
       </c>
       <c r="J36" s="14" t="s">
         <v>25</v>
@@ -1701,11 +1701,11 @@
         <v>0.1</v>
       </c>
       <c r="E37" s="16">
-        <v>9.9997891704508401E-2</v>
+        <v>9.9997857557748426E-2</v>
       </c>
       <c r="H37" s="16">
         <f t="shared" ref="H37:H41" si="0">B30*B$36+C30*B$37+D30*B$38+E30*B$39+F30*B$40+G30*B$41+I30</f>
-        <v>9.9997891704508401E-2</v>
+        <v>9.9997857557748426E-2</v>
       </c>
       <c r="K37" s="16">
         <f t="shared" ref="K37:K41" si="1">E37-H37</f>
@@ -1718,14 +1718,14 @@
         <v>-0.3</v>
       </c>
       <c r="E38" s="16">
-        <v>-0.33046470307044035</v>
+        <v>-0.33046470148141394</v>
       </c>
       <c r="F38">
         <v>2</v>
       </c>
       <c r="H38" s="16">
         <f t="shared" si="0"/>
-        <v>-0.33046470307044035</v>
+        <v>-0.33046470148141394</v>
       </c>
       <c r="K38" s="16">
         <f t="shared" si="1"/>
@@ -1737,11 +1737,11 @@
         <v>-0.2</v>
       </c>
       <c r="E39" s="16">
-        <v>-0.19999869073711646</v>
+        <v>-0.1999986695317941</v>
       </c>
       <c r="H39" s="16">
         <f t="shared" si="0"/>
-        <v>-0.19999869073711646</v>
+        <v>-0.1999986695317941</v>
       </c>
       <c r="K39" s="16">
         <f t="shared" si="1"/>
@@ -1753,11 +1753,11 @@
         <v>0.1</v>
       </c>
       <c r="E40" s="16">
-        <v>0.80706635416880779</v>
+        <v>0.80706628002800451</v>
       </c>
       <c r="H40" s="16">
         <f t="shared" si="0"/>
-        <v>0.80706635416880779</v>
+        <v>0.80706628002800451</v>
       </c>
       <c r="K40" s="16">
         <f t="shared" si="1"/>
@@ -1769,11 +1769,11 @@
         <v>0.2</v>
       </c>
       <c r="E41" s="17">
-        <v>0.20000348285010847</v>
+        <v>0.2000034938176917</v>
       </c>
       <c r="H41" s="17">
         <f t="shared" si="0"/>
-        <v>0.20000348285010847</v>
+        <v>0.2000034938176917</v>
       </c>
       <c r="K41" s="17">
         <f t="shared" si="1"/>

</xml_diff>